<commit_message>
universal usage of the filtered and attempted list
</commit_message>
<xml_diff>
--- a/data/championData.xlsx
+++ b/data/championData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\CODING\riftriddles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E08CC9-0025-4B7A-BB86-1D4043305C02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A82EF8-B134-4E01-A93C-DBDD87C216CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="185">
   <si>
     <t>Champion</t>
   </si>
@@ -556,6 +556,30 @@
   </si>
   <si>
     <t>Demacia</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Shurima</t>
+  </si>
+  <si>
+    <t>Icathia</t>
+  </si>
+  <si>
+    <t>Ranged</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>Vastayan</t>
   </si>
 </sst>
 </file>
@@ -884,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,231 +944,396 @@
       <c r="B2" t="s">
         <v>170</v>
       </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G3" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="C4" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="C7" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="C8" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="C10" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="C11" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="C13" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
+      <c r="C14" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
+      <c r="C15" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
+      <c r="C33" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
+      <c r="C35" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
+      <c r="C36" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
+      <c r="C37" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
+      <c r="C38" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
+      <c r="C40" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
+      <c r="C41" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
+      <c r="C42" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
+      <c r="C43" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
+      <c r="C44" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
+      <c r="C45" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
+      <c r="C46" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
+      <c r="C47" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -1169,584 +1358,932 @@
         <v>176</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C139" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C140" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C141" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C143" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C144" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C145" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C146" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C147" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C149" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C150" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C151" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C153" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C154" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C161" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
+      </c>
+      <c r="C164" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted some unnecessary files
</commit_message>
<xml_diff>
--- a/data/championData.xlsx
+++ b/data/championData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\CODING\riftriddles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549C6228-06C8-45DC-B357-8F62907CEF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D793D444-C30B-4580-8F4E-6B65289A0156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="597">
   <si>
     <t>Champion</t>
   </si>
@@ -1170,12 +1170,6 @@
     <t>⚡</t>
   </si>
   <si>
-    <t>🦗</t>
-  </si>
-  <si>
-    <t>🪰</t>
-  </si>
-  <si>
     <t>🏹</t>
   </si>
   <si>
@@ -1563,9 +1557,6 @@
     <t>🤻</t>
   </si>
   <si>
-    <t>👨🏽‍🔬</t>
-  </si>
-  <si>
     <t>🧔🏿‍♂️</t>
   </si>
   <si>
@@ -1707,9 +1698,6 @@
     <t>💸</t>
   </si>
   <si>
-    <t>👩‍💼</t>
-  </si>
-  <si>
     <t>🀄</t>
   </si>
   <si>
@@ -1822,6 +1810,12 @@
   </si>
   <si>
     <t>🤪</t>
+  </si>
+  <si>
+    <t>🧘🏻‍♂️</t>
+  </si>
+  <si>
+    <t>🧑🏾‍🔬</t>
   </si>
 </sst>
 </file>
@@ -2169,9 +2163,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L134" sqref="L134"/>
+      <selection pane="topRight" activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,7 +2277,7 @@
         <v>2011</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>296</v>
@@ -2292,7 +2286,7 @@
         <v>309</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2324,13 +2318,13 @@
         <v>297</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2359,13 +2353,13 @@
         <v>2021</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>312</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>378</v>
@@ -2444,7 +2438,7 @@
         <v>304</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2482,7 +2476,7 @@
         <v>307</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2549,7 +2543,7 @@
         <v>2019</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>312</v>
@@ -2590,10 +2584,10 @@
         <v>313</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>306</v>
@@ -2666,13 +2660,13 @@
         <v>313</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2742,13 +2736,13 @@
         <v>322</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>313</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2818,13 +2812,13 @@
         <v>309</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2856,10 +2850,10 @@
         <v>329</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>306</v>
@@ -2891,16 +2885,16 @@
         <v>2011</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2938,7 +2932,7 @@
         <v>331</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2976,7 +2970,7 @@
         <v>335</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3014,7 +3008,7 @@
         <v>324</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3046,10 +3040,10 @@
         <v>337</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>374</v>
@@ -3090,7 +3084,7 @@
         <v>300</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3119,16 +3113,16 @@
         <v>2012</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>339</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3198,7 +3192,7 @@
         <v>338</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>343</v>
@@ -3233,13 +3227,13 @@
         <v>2015</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>331</v>
@@ -3271,10 +3265,10 @@
         <v>2012</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>345</v>
@@ -3318,7 +3312,7 @@
         <v>310</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3347,10 +3341,10 @@
         <v>2010</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>326</v>
@@ -3388,7 +3382,7 @@
         <v>305</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>349</v>
@@ -3470,7 +3464,7 @@
         <v>353</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -3508,7 +3502,7 @@
         <v>357</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -3537,16 +3531,16 @@
         <v>2009</v>
       </c>
       <c r="I36" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="K36" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="J36" s="1" t="s">
-        <v>494</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>495</v>
-      </c>
       <c r="L36" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -3584,7 +3578,7 @@
         <v>351</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -3616,7 +3610,7 @@
         <v>337</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>359</v>
@@ -3651,16 +3645,16 @@
         <v>2010</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -3689,16 +3683,16 @@
         <v>2011</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -3736,7 +3730,7 @@
         <v>362</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -3771,10 +3765,10 @@
         <v>363</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -3806,10 +3800,10 @@
         <v>337</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>331</v>
@@ -3850,7 +3844,7 @@
         <v>352</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -3879,16 +3873,16 @@
         <v>2010</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3926,7 +3920,7 @@
         <v>360</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3955,16 +3949,16 @@
         <v>2009</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>358</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -4040,7 +4034,7 @@
         <v>370</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -4069,7 +4063,7 @@
         <v>2012</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>512</v>
+        <v>596</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>371</v>
@@ -4183,16 +4177,16 @@
         <v>2022</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>288</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -4221,16 +4215,16 @@
         <v>2018</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>322</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -4259,16 +4253,16 @@
         <v>2014</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>348</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -4300,13 +4294,13 @@
         <v>377</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -4338,7 +4332,7 @@
         <v>348</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>303</v>
@@ -4373,7 +4367,7 @@
         <v>2009</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>344</v>
@@ -4411,13 +4405,13 @@
         <v>2009</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>358</v>
@@ -4452,7 +4446,7 @@
         <v>378</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>288</v>
@@ -4493,10 +4487,10 @@
         <v>289</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -4534,7 +4528,7 @@
         <v>380</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -4563,16 +4557,16 @@
         <v>2012</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>381</v>
+        <v>393</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>322</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>382</v>
+        <v>512</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -4601,16 +4595,16 @@
         <v>2015</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -4639,13 +4633,13 @@
         <v>2016</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>337</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>288</v>
@@ -4680,13 +4674,13 @@
         <v>322</v>
       </c>
       <c r="J66" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="L66" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -4715,13 +4709,13 @@
         <v>2010</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>320</v>
@@ -4753,16 +4747,16 @@
         <v>2011</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -4791,16 +4785,16 @@
         <v>2011</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -4829,16 +4823,16 @@
         <v>2020</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>372</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -4870,13 +4864,13 @@
         <v>313</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>306</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -4905,7 +4899,7 @@
         <v>2013</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>312</v>
@@ -4914,7 +4908,7 @@
         <v>312</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -4949,7 +4943,7 @@
         <v>337</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>357</v>
@@ -4981,16 +4975,16 @@
         <v>2010</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>357</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -5022,10 +5016,10 @@
         <v>360</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>369</v>
@@ -5057,16 +5051,16 @@
         <v>2010</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>317</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -5104,7 +5098,7 @@
         <v>348</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -5133,16 +5127,13 @@
         <v>2009</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>541</v>
+        <v>595</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="L78" s="1" t="s">
-        <v>380</v>
+        <v>502</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -5171,16 +5162,16 @@
         <v>2023</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>309</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -5209,16 +5200,16 @@
         <v>2010</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -5256,7 +5247,7 @@
         <v>348</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -5285,13 +5276,13 @@
         <v>2009</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>310</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>301</v>
@@ -5323,16 +5314,16 @@
         <v>2012</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>352</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -5361,16 +5352,16 @@
         <v>2009</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>338</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -5399,16 +5390,16 @@
         <v>2012</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>352</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -5437,16 +5428,16 @@
         <v>2018</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>320</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -5478,13 +5469,13 @@
         <v>295</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -5516,10 +5507,10 @@
         <v>295</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>288</v>
@@ -5551,16 +5542,16 @@
         <v>2011</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>348</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -5589,7 +5580,7 @@
         <v>2009</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>359</v>
@@ -5598,7 +5589,7 @@
         <v>306</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -5671,10 +5662,10 @@
         <v>325</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -5703,10 +5694,10 @@
         <v>2017</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>309</v>
@@ -5741,10 +5732,10 @@
         <v>2010</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>288</v>
@@ -5785,10 +5776,10 @@
         <v>371</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -5817,13 +5808,13 @@
         <v>2018</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>348</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>352</v>
@@ -5864,7 +5855,7 @@
         <v>309</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -5893,16 +5884,16 @@
         <v>2013</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>295</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -5937,10 +5928,10 @@
         <v>379</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -5969,16 +5960,16 @@
         <v>2009</v>
       </c>
       <c r="I100" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="L100" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="K100" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="L100" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -6007,10 +5998,10 @@
         <v>2014</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>353</v>
@@ -6045,13 +6036,13 @@
         <v>2020</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L102" s="1" t="s">
         <v>295</v>
@@ -6083,16 +6074,16 @@
         <v>2022</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>560</v>
+        <v>461</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>342</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -6121,10 +6112,10 @@
         <v>2011</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>328</v>
@@ -6159,16 +6150,16 @@
         <v>2012</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J105" s="1" t="s">
         <v>335</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L105" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -6200,13 +6191,13 @@
         <v>288</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -6241,7 +6232,7 @@
         <v>325</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="L107" s="1" t="s">
         <v>374</v>
@@ -6273,16 +6264,16 @@
         <v>2009</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -6311,7 +6302,7 @@
         <v>2020</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="J109" s="1" t="s">
         <v>312</v>
@@ -6320,7 +6311,7 @@
         <v>312</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -6349,13 +6340,13 @@
         <v>2012</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="L110" s="1" t="s">
         <v>306</v>
@@ -6387,13 +6378,13 @@
         <v>2019</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>348</v>
@@ -6425,16 +6416,16 @@
         <v>2020</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K112" s="1" t="s">
         <v>321</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -6463,7 +6454,7 @@
         <v>2020</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J113" s="1" t="s">
         <v>300</v>
@@ -6472,7 +6463,7 @@
         <v>343</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -6501,16 +6492,16 @@
         <v>2009</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>340</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
@@ -6539,16 +6530,16 @@
         <v>2010</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
@@ -6577,13 +6568,13 @@
         <v>2011</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>423</v>
+        <v>314</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="L116" s="1" t="s">
         <v>309</v>
@@ -6615,16 +6606,16 @@
         <v>2009</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
@@ -6653,7 +6644,7 @@
         <v>2009</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="J118" s="1" t="s">
         <v>338</v>
@@ -6662,7 +6653,7 @@
         <v>334</v>
       </c>
       <c r="L118" s="1" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
@@ -6691,16 +6682,16 @@
         <v>2009</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
@@ -6729,13 +6720,13 @@
         <v>2011</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J120" s="1" t="s">
         <v>360</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="L120" s="1" t="s">
         <v>315</v>
@@ -6767,16 +6758,16 @@
         <v>2010</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J121" s="1" t="s">
         <v>321</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
@@ -6805,16 +6796,16 @@
         <v>2009</v>
       </c>
       <c r="I122" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K122" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="J122" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="K122" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="L122" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
@@ -6846,13 +6837,13 @@
         <v>340</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
@@ -6884,13 +6875,13 @@
         <v>301</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>357</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
@@ -6919,16 +6910,16 @@
         <v>2012</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
@@ -6957,16 +6948,16 @@
         <v>2015</v>
       </c>
       <c r="I126" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="K126" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="J126" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="K126" s="1" t="s">
-        <v>434</v>
-      </c>
       <c r="L126" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
@@ -6995,10 +6986,10 @@
         <v>2016</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="K127" s="1" t="s">
         <v>360</v>
@@ -7033,10 +7024,10 @@
         <v>2011</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="K128" s="1" t="s">
         <v>287</v>
@@ -7071,16 +7062,16 @@
         <v>2009</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -7112,13 +7103,13 @@
         <v>337</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
@@ -7150,7 +7141,7 @@
         <v>348</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K131" s="1" t="s">
         <v>301</v>
@@ -7191,7 +7182,7 @@
         <v>312</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>375</v>
@@ -7223,7 +7214,7 @@
         <v>2010</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J133" s="1" t="s">
         <v>313</v>
@@ -7232,7 +7223,7 @@
         <v>306</v>
       </c>
       <c r="L133" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -7261,7 +7252,7 @@
         <v>2009</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>288</v>
@@ -7270,7 +7261,7 @@
         <v>356</v>
       </c>
       <c r="L134" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
@@ -7299,16 +7290,16 @@
         <v>2009</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="L135" s="1" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -7337,16 +7328,16 @@
         <v>2009</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L136" s="1" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
@@ -7378,10 +7369,10 @@
         <v>311</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L137" s="1" t="s">
         <v>305</v>
@@ -7413,16 +7404,16 @@
         <v>2010</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K138" s="1" t="s">
         <v>301</v>
       </c>
       <c r="L138" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
@@ -7451,16 +7442,16 @@
         <v>2012</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K139" s="1" t="s">
         <v>340</v>
       </c>
       <c r="L139" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
@@ -7489,16 +7480,16 @@
         <v>2011</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="L140" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
@@ -7530,7 +7521,7 @@
         <v>337</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K141" s="1" t="s">
         <v>357</v>
@@ -7568,13 +7559,13 @@
         <v>322</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K142" s="1" t="s">
         <v>364</v>
       </c>
       <c r="L142" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
@@ -7606,10 +7597,10 @@
         <v>337</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="L143" s="1" t="s">
         <v>348</v>
@@ -7641,16 +7632,16 @@
         <v>2012</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="L144" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
@@ -7685,7 +7676,7 @@
         <v>348</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>288</v>
@@ -7755,16 +7746,16 @@
         <v>2010</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J147" s="1" t="s">
         <v>287</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="L147" s="1" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
@@ -7796,13 +7787,13 @@
         <v>311</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="K148" s="1" t="s">
         <v>380</v>
       </c>
       <c r="L148" s="1" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
@@ -7831,16 +7822,16 @@
         <v>2009</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>287</v>
       </c>
       <c r="L149" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
@@ -7869,16 +7860,16 @@
         <v>2011</v>
       </c>
       <c r="I150" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="K150" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="J150" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="K150" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="L150" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
@@ -7916,7 +7907,7 @@
         <v>379</v>
       </c>
       <c r="L151" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
@@ -7945,16 +7936,16 @@
         <v>2011</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="K152" s="1" t="s">
         <v>315</v>
       </c>
       <c r="L152" s="1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
@@ -7992,7 +7983,7 @@
         <v>288</v>
       </c>
       <c r="L153" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
@@ -8021,13 +8012,13 @@
         <v>2013</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J154" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>358</v>
@@ -8059,7 +8050,7 @@
         <v>2020</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J155" s="1" t="s">
         <v>288</v>
@@ -8068,7 +8059,7 @@
         <v>348</v>
       </c>
       <c r="L155" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
@@ -8097,10 +8088,10 @@
         <v>2011</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>303</v>
@@ -8135,13 +8126,13 @@
         <v>2019</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>315</v>
@@ -8173,16 +8164,16 @@
         <v>2013</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="J158" s="1" t="s">
         <v>342</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="L158" s="1" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
@@ -8211,16 +8202,16 @@
         <v>2012</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="L159" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
@@ -8255,10 +8246,10 @@
         <v>380</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="L160" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
@@ -8290,10 +8281,10 @@
         <v>337</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>375</v>
@@ -8325,16 +8316,16 @@
         <v>2009</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="L162" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
@@ -8366,13 +8357,13 @@
         <v>308</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K163" s="1" t="s">
         <v>315</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
@@ -8401,16 +8392,16 @@
         <v>2012</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="J164" s="1" t="s">
         <v>365</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "deleted some unnecessary files"
This reverts commit 15180ba16d0e41dd75e962d73d7f4b9590bed85b.
</commit_message>
<xml_diff>
--- a/data/championData.xlsx
+++ b/data/championData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\CODING\riftriddles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D793D444-C30B-4580-8F4E-6B65289A0156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549C6228-06C8-45DC-B357-8F62907CEF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1804" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="599">
   <si>
     <t>Champion</t>
   </si>
@@ -1170,6 +1170,12 @@
     <t>⚡</t>
   </si>
   <si>
+    <t>🦗</t>
+  </si>
+  <si>
+    <t>🪰</t>
+  </si>
+  <si>
     <t>🏹</t>
   </si>
   <si>
@@ -1557,6 +1563,9 @@
     <t>🤻</t>
   </si>
   <si>
+    <t>👨🏽‍🔬</t>
+  </si>
+  <si>
     <t>🧔🏿‍♂️</t>
   </si>
   <si>
@@ -1698,6 +1707,9 @@
     <t>💸</t>
   </si>
   <si>
+    <t>👩‍💼</t>
+  </si>
+  <si>
     <t>🀄</t>
   </si>
   <si>
@@ -1810,12 +1822,6 @@
   </si>
   <si>
     <t>🤪</t>
-  </si>
-  <si>
-    <t>🧘🏻‍♂️</t>
-  </si>
-  <si>
-    <t>🧑🏾‍🔬</t>
   </si>
 </sst>
 </file>
@@ -2163,9 +2169,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I50" sqref="I50"/>
+      <selection pane="topRight" activeCell="L134" sqref="L134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,7 +2283,7 @@
         <v>2011</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>296</v>
@@ -2286,7 +2292,7 @@
         <v>309</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2318,13 +2324,13 @@
         <v>297</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2353,13 +2359,13 @@
         <v>2021</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>312</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>378</v>
@@ -2438,7 +2444,7 @@
         <v>304</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2476,7 +2482,7 @@
         <v>307</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2543,7 +2549,7 @@
         <v>2019</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>312</v>
@@ -2584,10 +2590,10 @@
         <v>313</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>306</v>
@@ -2660,13 +2666,13 @@
         <v>313</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2736,13 +2742,13 @@
         <v>322</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>313</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2812,13 +2818,13 @@
         <v>309</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2850,10 +2856,10 @@
         <v>329</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>306</v>
@@ -2885,16 +2891,16 @@
         <v>2011</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2932,7 +2938,7 @@
         <v>331</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2970,7 +2976,7 @@
         <v>335</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3008,7 +3014,7 @@
         <v>324</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3040,10 +3046,10 @@
         <v>337</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>374</v>
@@ -3084,7 +3090,7 @@
         <v>300</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3113,16 +3119,16 @@
         <v>2012</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>339</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3192,7 +3198,7 @@
         <v>338</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>343</v>
@@ -3227,13 +3233,13 @@
         <v>2015</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="J28" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="K28" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>480</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>331</v>
@@ -3265,10 +3271,10 @@
         <v>2012</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>345</v>
@@ -3312,7 +3318,7 @@
         <v>310</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3341,10 +3347,10 @@
         <v>2010</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>326</v>
@@ -3382,7 +3388,7 @@
         <v>305</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>349</v>
@@ -3464,7 +3470,7 @@
         <v>353</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -3502,7 +3508,7 @@
         <v>357</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -3531,16 +3537,16 @@
         <v>2009</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -3578,7 +3584,7 @@
         <v>351</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -3610,7 +3616,7 @@
         <v>337</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>359</v>
@@ -3645,16 +3651,16 @@
         <v>2010</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -3683,16 +3689,16 @@
         <v>2011</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -3730,7 +3736,7 @@
         <v>362</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -3765,10 +3771,10 @@
         <v>363</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -3800,10 +3806,10 @@
         <v>337</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>331</v>
@@ -3844,7 +3850,7 @@
         <v>352</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -3873,16 +3879,16 @@
         <v>2010</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3920,7 +3926,7 @@
         <v>360</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3949,16 +3955,16 @@
         <v>2009</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>358</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -4034,7 +4040,7 @@
         <v>370</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -4063,7 +4069,7 @@
         <v>2012</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>596</v>
+        <v>512</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>371</v>
@@ -4177,16 +4183,16 @@
         <v>2022</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>288</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -4215,16 +4221,16 @@
         <v>2018</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>322</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -4253,16 +4259,16 @@
         <v>2014</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>348</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -4294,13 +4300,13 @@
         <v>377</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -4332,7 +4338,7 @@
         <v>348</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>303</v>
@@ -4367,7 +4373,7 @@
         <v>2009</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>344</v>
@@ -4405,13 +4411,13 @@
         <v>2009</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>358</v>
@@ -4446,7 +4452,7 @@
         <v>378</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>288</v>
@@ -4487,10 +4493,10 @@
         <v>289</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -4528,7 +4534,7 @@
         <v>380</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -4557,16 +4563,16 @@
         <v>2012</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>322</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>512</v>
+        <v>382</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -4595,16 +4601,16 @@
         <v>2015</v>
       </c>
       <c r="I64" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="K64" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="K64" s="1" t="s">
-        <v>381</v>
-      </c>
       <c r="L64" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -4633,13 +4639,13 @@
         <v>2016</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>337</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>288</v>
@@ -4674,13 +4680,13 @@
         <v>322</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -4709,13 +4715,13 @@
         <v>2010</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>320</v>
@@ -4747,16 +4753,16 @@
         <v>2011</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -4785,16 +4791,16 @@
         <v>2011</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -4823,16 +4829,16 @@
         <v>2020</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="J70" s="1" t="s">
         <v>372</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -4864,13 +4870,13 @@
         <v>313</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="K71" s="1" t="s">
         <v>306</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -4899,7 +4905,7 @@
         <v>2013</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>312</v>
@@ -4908,7 +4914,7 @@
         <v>312</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -4943,7 +4949,7 @@
         <v>337</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="L73" s="1" t="s">
         <v>357</v>
@@ -4975,16 +4981,16 @@
         <v>2010</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>357</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -5016,10 +5022,10 @@
         <v>360</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>369</v>
@@ -5051,16 +5057,16 @@
         <v>2010</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>317</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -5098,7 +5104,7 @@
         <v>348</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -5127,13 +5133,16 @@
         <v>2009</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>595</v>
+        <v>541</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>502</v>
+        <v>504</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -5162,16 +5171,16 @@
         <v>2023</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>309</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -5200,16 +5209,16 @@
         <v>2010</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -5247,7 +5256,7 @@
         <v>348</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -5276,13 +5285,13 @@
         <v>2009</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>310</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>301</v>
@@ -5314,16 +5323,16 @@
         <v>2012</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="K83" s="1" t="s">
         <v>352</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -5352,16 +5361,16 @@
         <v>2009</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="K84" s="1" t="s">
         <v>338</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -5390,16 +5399,16 @@
         <v>2012</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>352</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -5428,16 +5437,16 @@
         <v>2018</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>320</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -5469,13 +5478,13 @@
         <v>295</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -5507,10 +5516,10 @@
         <v>295</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>288</v>
@@ -5542,16 +5551,16 @@
         <v>2011</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>348</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -5580,7 +5589,7 @@
         <v>2009</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>359</v>
@@ -5589,7 +5598,7 @@
         <v>306</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -5662,10 +5671,10 @@
         <v>325</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -5694,10 +5703,10 @@
         <v>2017</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>309</v>
@@ -5732,10 +5741,10 @@
         <v>2010</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>288</v>
@@ -5776,10 +5785,10 @@
         <v>371</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -5808,13 +5817,13 @@
         <v>2018</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>348</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>352</v>
@@ -5855,7 +5864,7 @@
         <v>309</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -5884,16 +5893,16 @@
         <v>2013</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>295</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -5928,10 +5937,10 @@
         <v>379</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -5960,16 +5969,16 @@
         <v>2009</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -5998,10 +6007,10 @@
         <v>2014</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="K101" s="1" t="s">
         <v>353</v>
@@ -6036,13 +6045,13 @@
         <v>2020</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="L102" s="1" t="s">
         <v>295</v>
@@ -6074,16 +6083,16 @@
         <v>2022</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>461</v>
+        <v>560</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>342</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -6112,10 +6121,10 @@
         <v>2011</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>328</v>
@@ -6150,16 +6159,16 @@
         <v>2012</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="J105" s="1" t="s">
         <v>335</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="L105" s="1" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -6191,13 +6200,13 @@
         <v>288</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -6232,7 +6241,7 @@
         <v>325</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="L107" s="1" t="s">
         <v>374</v>
@@ -6264,16 +6273,16 @@
         <v>2009</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -6302,7 +6311,7 @@
         <v>2020</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="J109" s="1" t="s">
         <v>312</v>
@@ -6311,7 +6320,7 @@
         <v>312</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -6340,13 +6349,13 @@
         <v>2012</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="L110" s="1" t="s">
         <v>306</v>
@@ -6378,13 +6387,13 @@
         <v>2019</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>312</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="L111" s="1" t="s">
         <v>348</v>
@@ -6416,16 +6425,16 @@
         <v>2020</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="K112" s="1" t="s">
         <v>321</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -6454,7 +6463,7 @@
         <v>2020</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="J113" s="1" t="s">
         <v>300</v>
@@ -6463,7 +6472,7 @@
         <v>343</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -6492,16 +6501,16 @@
         <v>2009</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J114" s="1" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="K114" s="1" t="s">
         <v>340</v>
       </c>
       <c r="L114" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
@@ -6530,16 +6539,16 @@
         <v>2010</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
@@ -6568,13 +6577,13 @@
         <v>2011</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>314</v>
+        <v>423</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="L116" s="1" t="s">
         <v>309</v>
@@ -6606,16 +6615,16 @@
         <v>2009</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
@@ -6644,7 +6653,7 @@
         <v>2009</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="J118" s="1" t="s">
         <v>338</v>
@@ -6653,7 +6662,7 @@
         <v>334</v>
       </c>
       <c r="L118" s="1" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
@@ -6682,16 +6691,16 @@
         <v>2009</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
@@ -6720,13 +6729,13 @@
         <v>2011</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="J120" s="1" t="s">
         <v>360</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="L120" s="1" t="s">
         <v>315</v>
@@ -6758,16 +6767,16 @@
         <v>2010</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="J121" s="1" t="s">
         <v>321</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
@@ -6796,16 +6805,16 @@
         <v>2009</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="J122" s="1" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="L122" s="1" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
@@ -6837,13 +6846,13 @@
         <v>340</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
@@ -6875,13 +6884,13 @@
         <v>301</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="K124" s="1" t="s">
         <v>357</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
@@ -6910,16 +6919,16 @@
         <v>2012</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
@@ -6948,16 +6957,16 @@
         <v>2015</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="J126" s="1" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="L126" s="1" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
@@ -6986,10 +6995,10 @@
         <v>2016</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="K127" s="1" t="s">
         <v>360</v>
@@ -7024,10 +7033,10 @@
         <v>2011</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="K128" s="1" t="s">
         <v>287</v>
@@ -7062,16 +7071,16 @@
         <v>2009</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -7103,13 +7112,13 @@
         <v>337</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
@@ -7141,7 +7150,7 @@
         <v>348</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="K131" s="1" t="s">
         <v>301</v>
@@ -7182,7 +7191,7 @@
         <v>312</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="L132" s="1" t="s">
         <v>375</v>
@@ -7214,7 +7223,7 @@
         <v>2010</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="J133" s="1" t="s">
         <v>313</v>
@@ -7223,7 +7232,7 @@
         <v>306</v>
       </c>
       <c r="L133" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -7252,7 +7261,7 @@
         <v>2009</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>288</v>
@@ -7261,7 +7270,7 @@
         <v>356</v>
       </c>
       <c r="L134" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
@@ -7290,16 +7299,16 @@
         <v>2009</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="L135" s="1" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -7328,16 +7337,16 @@
         <v>2009</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="L136" s="1" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
@@ -7369,10 +7378,10 @@
         <v>311</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="L137" s="1" t="s">
         <v>305</v>
@@ -7404,16 +7413,16 @@
         <v>2010</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>575</v>
+        <v>579</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="K138" s="1" t="s">
         <v>301</v>
       </c>
       <c r="L138" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
@@ -7442,16 +7451,16 @@
         <v>2012</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="K139" s="1" t="s">
         <v>340</v>
       </c>
       <c r="L139" s="1" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
@@ -7480,16 +7489,16 @@
         <v>2011</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="L140" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
@@ -7521,7 +7530,7 @@
         <v>337</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="K141" s="1" t="s">
         <v>357</v>
@@ -7559,13 +7568,13 @@
         <v>322</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="K142" s="1" t="s">
         <v>364</v>
       </c>
       <c r="L142" s="1" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
@@ -7597,10 +7606,10 @@
         <v>337</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="L143" s="1" t="s">
         <v>348</v>
@@ -7632,16 +7641,16 @@
         <v>2012</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="L144" s="1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
@@ -7676,7 +7685,7 @@
         <v>348</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>288</v>
@@ -7746,16 +7755,16 @@
         <v>2010</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J147" s="1" t="s">
         <v>287</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="L147" s="1" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
@@ -7787,13 +7796,13 @@
         <v>311</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="K148" s="1" t="s">
         <v>380</v>
       </c>
       <c r="L148" s="1" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
@@ -7822,16 +7831,16 @@
         <v>2009</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>287</v>
       </c>
       <c r="L149" s="1" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
@@ -7860,16 +7869,16 @@
         <v>2011</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L150" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
@@ -7907,7 +7916,7 @@
         <v>379</v>
       </c>
       <c r="L151" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
@@ -7936,16 +7945,16 @@
         <v>2011</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="K152" s="1" t="s">
         <v>315</v>
       </c>
       <c r="L152" s="1" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
@@ -7983,7 +7992,7 @@
         <v>288</v>
       </c>
       <c r="L153" s="1" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
@@ -8012,13 +8021,13 @@
         <v>2013</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="J154" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="L154" s="1" t="s">
         <v>358</v>
@@ -8050,7 +8059,7 @@
         <v>2020</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="J155" s="1" t="s">
         <v>288</v>
@@ -8059,7 +8068,7 @@
         <v>348</v>
       </c>
       <c r="L155" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
@@ -8088,10 +8097,10 @@
         <v>2011</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="K156" s="1" t="s">
         <v>303</v>
@@ -8126,13 +8135,13 @@
         <v>2019</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="L157" s="1" t="s">
         <v>315</v>
@@ -8164,16 +8173,16 @@
         <v>2013</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="J158" s="1" t="s">
         <v>342</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="L158" s="1" t="s">
-        <v>586</v>
+        <v>590</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
@@ -8202,16 +8211,16 @@
         <v>2012</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="L159" s="1" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
@@ -8246,10 +8255,10 @@
         <v>380</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="L160" s="1" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
@@ -8281,10 +8290,10 @@
         <v>337</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="L161" s="1" t="s">
         <v>375</v>
@@ -8316,16 +8325,16 @@
         <v>2009</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="L162" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
@@ -8357,13 +8366,13 @@
         <v>308</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="K163" s="1" t="s">
         <v>315</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
@@ -8392,16 +8401,16 @@
         <v>2012</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="J164" s="1" t="s">
         <v>365</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>585</v>
+        <v>589</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reinstalled all the packages
</commit_message>
<xml_diff>
--- a/data/championData.xlsx
+++ b/data/championData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\CODING\riftriddles\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F98438-DEE7-433A-8A39-03725C10A6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF7C79B-429D-447E-A107-AE1D626A4561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6495" yWindow="2730" windowWidth="19560" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1805" uniqueCount="605">
   <si>
     <t>Champion</t>
   </si>
@@ -921,9 +921,6 @@
     <t>🥷</t>
   </si>
   <si>
-    <t>🧔</t>
-  </si>
-  <si>
     <t>🐂</t>
   </si>
   <si>
@@ -1158,9 +1155,6 @@
     <t>🧟</t>
   </si>
   <si>
-    <t>🧘</t>
-  </si>
-  <si>
     <t>😇</t>
   </si>
   <si>
@@ -1497,9 +1491,6 @@
     <t>🗺️</t>
   </si>
   <si>
-    <t>👱‍♂️</t>
-  </si>
-  <si>
     <t>🎃</t>
   </si>
   <si>
@@ -1542,12 +1533,6 @@
     <t>🥋</t>
   </si>
   <si>
-    <t>💃</t>
-  </si>
-  <si>
-    <t>🙍🏻‍♀️</t>
-  </si>
-  <si>
     <t>🔹</t>
   </si>
   <si>
@@ -1560,9 +1545,6 @@
     <t>🌪️</t>
   </si>
   <si>
-    <t>🤻</t>
-  </si>
-  <si>
     <t>👨🏽‍🔬</t>
   </si>
   <si>
@@ -1584,9 +1566,6 @@
     <t>🌨️</t>
   </si>
   <si>
-    <t>🧟‍♀️</t>
-  </si>
-  <si>
     <t>🪷</t>
   </si>
   <si>
@@ -1707,9 +1686,6 @@
     <t>💸</t>
   </si>
   <si>
-    <t>👩‍💼</t>
-  </si>
-  <si>
     <t>🀄</t>
   </si>
   <si>
@@ -1822,6 +1798,48 @@
   </si>
   <si>
     <t>🤪</t>
+  </si>
+  <si>
+    <t>🚁</t>
+  </si>
+  <si>
+    <t>👧🏼</t>
+  </si>
+  <si>
+    <t>💪🏽</t>
+  </si>
+  <si>
+    <t>🫂</t>
+  </si>
+  <si>
+    <t>🧙🏻‍♀️</t>
+  </si>
+  <si>
+    <t>👭🏻</t>
+  </si>
+  <si>
+    <t>🧙🏿‍♂️</t>
+  </si>
+  <si>
+    <t>🦹🏽‍♀️</t>
+  </si>
+  <si>
+    <t>🧘🏽‍♀️</t>
+  </si>
+  <si>
+    <t>🗜️</t>
+  </si>
+  <si>
+    <t>💃🏻</t>
+  </si>
+  <si>
+    <t>🧔🏼‍♂️</t>
+  </si>
+  <si>
+    <t>👦🏼</t>
+  </si>
+  <si>
+    <t>🤴🏻</t>
   </si>
 </sst>
 </file>
@@ -2169,9 +2187,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K15" sqref="K15"/>
+      <selection pane="topRight" activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,16 +2301,16 @@
         <v>2011</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>296</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2324,13 +2342,13 @@
         <v>297</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="L4" s="4" t="s">
         <v>464</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2359,16 +2377,16 @@
         <v>2021</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2397,16 +2415,16 @@
         <v>2009</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>301</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2435,16 +2453,16 @@
         <v>2009</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>304</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2473,16 +2491,16 @@
         <v>2009</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>307</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2511,16 +2529,16 @@
         <v>2009</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2549,16 +2567,16 @@
         <v>2019</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2587,16 +2605,16 @@
         <v>2009</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2625,16 +2643,16 @@
         <v>2016</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>316</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2663,16 +2681,16 @@
         <v>2014</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2701,16 +2719,16 @@
         <v>2015</v>
       </c>
       <c r="I14" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>318</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2739,16 +2757,16 @@
         <v>2022</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2777,16 +2795,16 @@
         <v>2009</v>
       </c>
       <c r="I16" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>327</v>
-      </c>
       <c r="L16" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2815,16 +2833,16 @@
         <v>2011</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2853,16 +2871,16 @@
         <v>2014</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2891,16 +2909,16 @@
         <v>2011</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2929,16 +2947,16 @@
         <v>2016</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="L20" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2967,16 +2985,16 @@
         <v>2010</v>
       </c>
       <c r="I21" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>335</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3005,16 +3023,16 @@
         <v>2009</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3043,16 +3061,16 @@
         <v>2009</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3081,16 +3099,16 @@
         <v>2012</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>287</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>300</v>
+        <v>593</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3119,16 +3137,16 @@
         <v>2012</v>
       </c>
       <c r="I25" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>481</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3157,16 +3175,16 @@
         <v>2009</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J26" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>342</v>
-      </c>
       <c r="L26" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -3195,13 +3213,13 @@
         <v>2012</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>287</v>
@@ -3233,16 +3251,16 @@
         <v>2015</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3271,16 +3289,16 @@
         <v>2012</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -3309,16 +3327,16 @@
         <v>2009</v>
       </c>
       <c r="I30" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="J30" s="1" t="s">
-        <v>347</v>
-      </c>
       <c r="K30" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -3347,16 +3365,16 @@
         <v>2010</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>490</v>
+        <v>603</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -3385,16 +3403,16 @@
         <v>2009</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3423,16 +3441,16 @@
         <v>2012</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>295</v>
+        <v>461</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -3461,16 +3479,16 @@
         <v>2011</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
@@ -3499,16 +3517,16 @@
         <v>2010</v>
       </c>
       <c r="I35" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>357</v>
-      </c>
       <c r="L35" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -3537,16 +3555,16 @@
         <v>2009</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -3575,16 +3593,16 @@
         <v>2010</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
@@ -3613,16 +3631,16 @@
         <v>2014</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K38" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="L38" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="L38" s="1" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -3651,16 +3669,16 @@
         <v>2010</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
@@ -3689,16 +3707,16 @@
         <v>2011</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -3727,16 +3745,16 @@
         <v>2021</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>308</v>
+        <v>592</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
@@ -3765,16 +3783,16 @@
         <v>2012</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
@@ -3803,16 +3821,16 @@
         <v>2009</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
@@ -3841,16 +3859,16 @@
         <v>2015</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>300</v>
+        <v>593</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
@@ -3879,16 +3897,16 @@
         <v>2010</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>506</v>
+        <v>461</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>505</v>
+        <v>601</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -3917,16 +3935,16 @@
         <v>2016</v>
       </c>
       <c r="I46" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="J46" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>366</v>
-      </c>
       <c r="K46" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -3955,16 +3973,16 @@
         <v>2009</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
@@ -3993,16 +4011,16 @@
         <v>2011</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>313</v>
+        <v>604</v>
       </c>
       <c r="J48" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="L48" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -4031,16 +4049,16 @@
         <v>2009</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>511</v>
+        <v>591</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -4069,16 +4087,16 @@
         <v>2012</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -4107,16 +4125,16 @@
         <v>2016</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K51" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="L51" s="1" t="s">
         <v>372</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -4145,16 +4163,16 @@
         <v>2013</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K52" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="L52" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="L52" s="1" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -4183,16 +4201,16 @@
         <v>2022</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>288</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -4221,16 +4239,16 @@
         <v>2018</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>506</v>
+        <v>461</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
@@ -4259,16 +4277,16 @@
         <v>2014</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>519</v>
+        <v>347</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>348</v>
+        <v>594</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -4297,16 +4315,16 @@
         <v>2011</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>377</v>
+        <v>599</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -4335,16 +4353,16 @@
         <v>2009</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -4373,16 +4391,16 @@
         <v>2009</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -4411,16 +4429,16 @@
         <v>2009</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
@@ -4449,16 +4467,16 @@
         <v>2009</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>288</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -4493,10 +4511,10 @@
         <v>289</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -4525,16 +4543,16 @@
         <v>2010</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>297</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -4563,16 +4581,16 @@
         <v>2012</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -4601,16 +4619,16 @@
         <v>2015</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -4639,13 +4657,13 @@
         <v>2016</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>288</v>
@@ -4677,16 +4695,16 @@
         <v>2010</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J66" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="L66" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="K66" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -4715,16 +4733,16 @@
         <v>2010</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -4753,16 +4771,16 @@
         <v>2011</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -4791,16 +4809,16 @@
         <v>2011</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -4829,16 +4847,16 @@
         <v>2020</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -4867,16 +4885,16 @@
         <v>2013</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
@@ -4905,16 +4923,16 @@
         <v>2013</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
@@ -4943,16 +4961,16 @@
         <v>2012</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
@@ -4981,16 +4999,16 @@
         <v>2010</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -5019,16 +5037,16 @@
         <v>2009</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -5057,16 +5075,16 @@
         <v>2010</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -5095,16 +5113,16 @@
         <v>2011</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -5133,16 +5151,16 @@
         <v>2009</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -5171,16 +5189,16 @@
         <v>2023</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -5209,16 +5227,16 @@
         <v>2010</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -5247,16 +5265,16 @@
         <v>2010</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.25">
@@ -5285,16 +5303,16 @@
         <v>2009</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -5323,16 +5341,16 @@
         <v>2012</v>
       </c>
       <c r="I83" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="L83" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="K83" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.25">
@@ -5361,16 +5379,16 @@
         <v>2009</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -5399,16 +5417,16 @@
         <v>2012</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L85" s="1" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -5437,16 +5455,16 @@
         <v>2018</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>444</v>
+        <v>596</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
@@ -5478,13 +5496,13 @@
         <v>295</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.25">
@@ -5516,10 +5534,10 @@
         <v>295</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>288</v>
@@ -5551,16 +5569,16 @@
         <v>2011</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
@@ -5589,16 +5607,16 @@
         <v>2009</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -5627,16 +5645,16 @@
         <v>2010</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>298</v>
+        <v>602</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.25">
@@ -5665,16 +5683,16 @@
         <v>2011</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K92" s="1" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -5703,16 +5721,16 @@
         <v>2017</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -5741,16 +5759,16 @@
         <v>2010</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K94" s="1" t="s">
         <v>288</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
@@ -5779,16 +5797,16 @@
         <v>2010</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K95" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
@@ -5817,16 +5835,16 @@
         <v>2018</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="J96" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -5855,16 +5873,16 @@
         <v>2019</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J97" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K97" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -5893,16 +5911,16 @@
         <v>2013</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>295</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.25">
@@ -5931,16 +5949,16 @@
         <v>2017</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J99" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -5969,16 +5987,16 @@
         <v>2009</v>
       </c>
       <c r="I100" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="L100" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="K100" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="L100" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -6007,16 +6025,16 @@
         <v>2014</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J101" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.25">
@@ -6045,16 +6063,16 @@
         <v>2020</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="J102" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L102" s="1" t="s">
-        <v>295</v>
+        <v>600</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.25">
@@ -6083,16 +6101,16 @@
         <v>2022</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>560</v>
+        <v>598</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="K103" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -6121,16 +6139,16 @@
         <v>2011</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="L104" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
@@ -6159,16 +6177,16 @@
         <v>2012</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K105" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L105" s="1" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.25">
@@ -6200,13 +6218,13 @@
         <v>288</v>
       </c>
       <c r="J106" s="1" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="K106" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L106" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -6235,16 +6253,16 @@
         <v>2011</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K107" s="1" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="L107" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.25">
@@ -6273,16 +6291,16 @@
         <v>2009</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="K108" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -6311,16 +6329,16 @@
         <v>2020</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L109" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -6349,16 +6367,16 @@
         <v>2012</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J110" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="L110" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
@@ -6387,16 +6405,16 @@
         <v>2019</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="L111" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.25">
@@ -6425,16 +6443,16 @@
         <v>2020</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="J112" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L112" s="1" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
@@ -6463,16 +6481,16 @@
         <v>2020</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
@@ -6501,16 +6519,16 @@
         <v>2009</v>
       </c>
       <c r="I114" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="L114" s="1" t="s">
         <v>420</v>
-      </c>
-      <c r="J114" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="K114" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="L114" s="1" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
@@ -6539,16 +6557,16 @@
         <v>2010</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L115" s="1" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
@@ -6577,16 +6595,16 @@
         <v>2011</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="J116" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="L116" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
@@ -6615,16 +6633,16 @@
         <v>2009</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="L117" s="1" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
@@ -6653,16 +6671,16 @@
         <v>2009</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="J118" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="L118" s="1" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
@@ -6691,16 +6709,16 @@
         <v>2009</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="L119" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
@@ -6729,16 +6747,16 @@
         <v>2011</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J120" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="L120" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
@@ -6767,16 +6785,16 @@
         <v>2010</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="J121" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
     </row>
     <row r="122" spans="1:12" x14ac:dyDescent="0.25">
@@ -6805,16 +6823,16 @@
         <v>2009</v>
       </c>
       <c r="I122" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="J122" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="K122" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="J122" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="K122" s="1" t="s">
-        <v>431</v>
-      </c>
       <c r="L122" s="1" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="123" spans="1:12" x14ac:dyDescent="0.25">
@@ -6843,16 +6861,16 @@
         <v>2010</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="L123" s="1" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
     </row>
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
@@ -6881,16 +6899,16 @@
         <v>2019</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L124" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="125" spans="1:12" x14ac:dyDescent="0.25">
@@ -6919,16 +6937,16 @@
         <v>2012</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>537</v>
+        <v>595</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="L125" s="1" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.25">
@@ -6957,16 +6975,16 @@
         <v>2015</v>
       </c>
       <c r="I126" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="K126" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="J126" s="1" t="s">
-        <v>575</v>
-      </c>
-      <c r="K126" s="1" t="s">
-        <v>434</v>
-      </c>
       <c r="L126" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.25">
@@ -6995,16 +7013,16 @@
         <v>2016</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="J127" s="1" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L127" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="128" spans="1:12" x14ac:dyDescent="0.25">
@@ -7033,10 +7051,10 @@
         <v>2011</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J128" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="K128" s="1" t="s">
         <v>287</v>
@@ -7071,16 +7089,16 @@
         <v>2009</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="J129" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="L129" s="1" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="130" spans="1:12" x14ac:dyDescent="0.25">
@@ -7109,16 +7127,16 @@
         <v>2009</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J130" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L130" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.25">
@@ -7147,16 +7165,16 @@
         <v>2013</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="J131" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L131" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
@@ -7185,16 +7203,16 @@
         <v>2009</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L132" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.25">
@@ -7223,16 +7241,16 @@
         <v>2010</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J133" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="L133" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="134" spans="1:12" x14ac:dyDescent="0.25">
@@ -7261,16 +7279,16 @@
         <v>2009</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L134" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
@@ -7299,16 +7317,16 @@
         <v>2009</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="J135" s="1" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="L135" s="1" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
     </row>
     <row r="136" spans="1:12" x14ac:dyDescent="0.25">
@@ -7337,16 +7355,16 @@
         <v>2009</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J136" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K136" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L136" s="1" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="137" spans="1:12" x14ac:dyDescent="0.25">
@@ -7375,16 +7393,16 @@
         <v>2009</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J137" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L137" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="138" spans="1:12" x14ac:dyDescent="0.25">
@@ -7413,16 +7431,16 @@
         <v>2010</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L138" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="139" spans="1:12" x14ac:dyDescent="0.25">
@@ -7451,16 +7469,16 @@
         <v>2012</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J139" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L139" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
@@ -7489,16 +7507,16 @@
         <v>2011</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="L140" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="141" spans="1:12" x14ac:dyDescent="0.25">
@@ -7527,16 +7545,16 @@
         <v>2009</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J141" s="1" t="s">
-        <v>393</v>
+        <v>597</v>
       </c>
       <c r="K141" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="L141" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="L141" s="1" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="142" spans="1:12" x14ac:dyDescent="0.25">
@@ -7565,16 +7583,16 @@
         <v>2014</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J142" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L142" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
@@ -7603,16 +7621,16 @@
         <v>2021</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J143" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="L143" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
@@ -7641,16 +7659,16 @@
         <v>2012</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="L144" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
@@ -7679,13 +7697,13 @@
         <v>2021</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="L145" s="1" t="s">
         <v>288</v>
@@ -7717,16 +7735,16 @@
         <v>2011</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L146" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
@@ -7755,16 +7773,16 @@
         <v>2010</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="J147" s="1" t="s">
         <v>287</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="L147" s="1" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
@@ -7793,16 +7811,16 @@
         <v>2011</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J148" s="1" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L148" s="1" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
     </row>
     <row r="149" spans="1:12" x14ac:dyDescent="0.25">
@@ -7831,16 +7849,16 @@
         <v>2009</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J149" s="1" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="K149" s="1" t="s">
         <v>287</v>
       </c>
       <c r="L149" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
@@ -7869,16 +7887,16 @@
         <v>2011</v>
       </c>
       <c r="I150" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J150" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="K150" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="J150" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="K150" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="L150" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="151" spans="1:12" x14ac:dyDescent="0.25">
@@ -7910,13 +7928,13 @@
         <v>295</v>
       </c>
       <c r="J151" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="L151" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="152" spans="1:12" x14ac:dyDescent="0.25">
@@ -7945,16 +7963,16 @@
         <v>2011</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="J152" s="1" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L152" s="1" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="153" spans="1:12" x14ac:dyDescent="0.25">
@@ -7983,16 +8001,16 @@
         <v>2010</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="J153" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K153" s="1" t="s">
         <v>288</v>
       </c>
       <c r="L153" s="1" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
     </row>
     <row r="154" spans="1:12" x14ac:dyDescent="0.25">
@@ -8021,16 +8039,16 @@
         <v>2013</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J154" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="L154" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="155" spans="1:12" x14ac:dyDescent="0.25">
@@ -8059,16 +8077,16 @@
         <v>2020</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J155" s="1" t="s">
         <v>288</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L155" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
@@ -8097,16 +8115,16 @@
         <v>2011</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="J156" s="1" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="L156" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="157" spans="1:12" x14ac:dyDescent="0.25">
@@ -8135,16 +8153,16 @@
         <v>2019</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J157" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="L157" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
@@ -8173,16 +8191,16 @@
         <v>2013</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="J158" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="L158" s="1" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
     </row>
     <row r="159" spans="1:12" x14ac:dyDescent="0.25">
@@ -8211,16 +8229,16 @@
         <v>2012</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="J159" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K159" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="L159" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
@@ -8249,16 +8267,16 @@
         <v>2022</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="L160" s="1" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="161" spans="1:12" x14ac:dyDescent="0.25">
@@ -8287,16 +8305,16 @@
         <v>2012</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J161" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K161" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="L161" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="162" spans="1:12" x14ac:dyDescent="0.25">
@@ -8325,16 +8343,16 @@
         <v>2009</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="J162" s="1" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="K162" s="1" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="L162" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.25">
@@ -8363,16 +8381,16 @@
         <v>2017</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J163" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L163" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.25">
@@ -8401,16 +8419,16 @@
         <v>2012</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="J164" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K164" s="1" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="L164" s="1" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>